<commit_message>
zaw - login - testing
</commit_message>
<xml_diff>
--- a/documentation/04_テスト/01_単体テスト/Backend/テストケース番号作成方法.xlsx
+++ b/documentation/04_テスト/01_単体テスト/Backend/テストケース番号作成方法.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>01　-　管理者</t>
   </si>
   <si>
-    <t>01　-　利用者</t>
+    <t>02　-　利用者</t>
+  </si>
+  <si>
+    <t>03　-　一般</t>
   </si>
   <si>
     <t>001　-　本一覧</t>
@@ -56,6 +59,15 @@
   </si>
   <si>
     <t>012　-　請求先と支払い削除</t>
+  </si>
+  <si>
+    <t>013　-　ログイン</t>
+  </si>
+  <si>
+    <t>014　-　アカウント登録</t>
+  </si>
+  <si>
+    <t>015　-　プロフィール</t>
   </si>
   <si>
     <t>001 - テストケース番号</t>
@@ -72,10 +84,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -86,55 +98,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -154,6 +130,81 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -163,15 +214,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,36 +222,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -217,14 +236,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,181 +257,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,41 +442,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -483,17 +460,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,9 +495,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,15 +545,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -551,130 +563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -999,10 +1011,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B3:B26"/>
+  <dimension ref="B3:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1017,8 +1029,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1077,19 +1089,39 @@
         <v>13</v>
       </c>
     </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zaw - testing - shoppingCart - commit
</commit_message>
<xml_diff>
--- a/documentation/04_テスト/01_単体テスト/Backend/テストケース番号作成方法.xlsx
+++ b/documentation/04_テスト/01_単体テスト/Backend/テストケース番号作成方法.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>01　-　管理者</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>015　-　プロフィール</t>
+  </si>
+  <si>
+    <t>016　-　ショッピングカート</t>
   </si>
   <si>
     <t>001 - テストケース番号</t>
@@ -85,9 +88,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -95,14 +98,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -114,11 +109,101 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -130,38 +215,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,74 +240,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,43 +254,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,43 +392,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,91 +422,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,21 +445,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -478,17 +466,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -504,17 +492,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,7 +548,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -563,130 +566,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +1017,7 @@
   <dimension ref="B3:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1109,19 +1112,24 @@
         <v>17</v>
       </c>
     </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zaw - testing - checkout - commit
</commit_message>
<xml_diff>
--- a/documentation/04_テスト/01_単体テスト/Backend/テストケース番号作成方法.xlsx
+++ b/documentation/04_テスト/01_単体テスト/Backend/テストケース番号作成方法.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>01　-　管理者</t>
   </si>
@@ -73,7 +73,10 @@
     <t>016　-　ショッピングカート</t>
   </si>
   <si>
-    <t>017　-　ユーザ</t>
+    <t>017　-　ユーザー</t>
+  </si>
+  <si>
+    <t>018　-　チェックアウト</t>
   </si>
   <si>
     <t>001 - テストケース番号</t>
@@ -90,9 +93,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -104,9 +107,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -119,6 +136,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -128,30 +152,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -173,10 +182,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -188,31 +206,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,29 +245,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,13 +260,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,151 +392,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,63 +451,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -540,6 +486,63 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -551,15 +554,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -569,130 +572,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1017,10 +1020,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B3:B32"/>
+  <dimension ref="B3:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1125,19 +1128,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="s">
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>